<commit_message>
made changes in the folder
</commit_message>
<xml_diff>
--- a/food_survey.xlsx
+++ b/food_survey.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christopherjrgalgo/Desktop/dsprojects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92C5695C-4B65-154C-971E-61C6093FDE2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12568922-A775-E24E-9F10-3929E6CDFAAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12220" yWindow="500" windowWidth="16580" windowHeight="16580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2779,9 +2779,6 @@
     <t>more available healthy foods  malls</t>
   </si>
   <si>
-    <t>intense use pesticides preservatives right from the start of production,  processed or cultured.</t>
-  </si>
-  <si>
     <t>healthy food become more expensive, with labels, well packaging, branded and certified.</t>
   </si>
   <si>
@@ -2815,9 +2812,6 @@
     <t>preservatives</t>
   </si>
   <si>
-    <t xml:space="preserve"> nutritious good health </t>
-  </si>
-  <si>
     <t>Healthy body  strong  body resistance</t>
   </si>
   <si>
@@ -3041,6 +3035,12 @@
   </si>
   <si>
     <t>benefits</t>
+  </si>
+  <si>
+    <t>intense use pesticides preservatives right from the start of production,  processed or cultured</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nutritious good health </t>
   </si>
 </sst>
 </file>
@@ -3299,8 +3299,8 @@
   </sheetPr>
   <dimension ref="A1:R139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M106" workbookViewId="0">
-      <selection activeCell="N140" sqref="N140"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="N149" sqref="N149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4340,7 +4340,7 @@
         <v>163</v>
       </c>
       <c r="N19" t="s">
-        <v>913</v>
+        <v>999</v>
       </c>
       <c r="O19" t="s">
         <v>164</v>
@@ -4396,7 +4396,7 @@
         <v>172</v>
       </c>
       <c r="N20" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="O20" t="s">
         <v>173</v>
@@ -4452,7 +4452,7 @@
         <v>180</v>
       </c>
       <c r="N21" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="O21" t="s">
         <v>181</v>
@@ -4508,7 +4508,7 @@
         <v>124</v>
       </c>
       <c r="N22" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="O22" t="s">
         <v>187</v>
@@ -4617,7 +4617,7 @@
         <v>124</v>
       </c>
       <c r="N24" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="O24" t="s">
         <v>199</v>
@@ -4726,7 +4726,7 @@
         <v>219</v>
       </c>
       <c r="N26" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="O26" t="s">
         <v>220</v>
@@ -4782,7 +4782,7 @@
         <v>225</v>
       </c>
       <c r="N27" t="s">
-        <v>939</v>
+        <v>937</v>
       </c>
       <c r="O27" t="s">
         <v>226</v>
@@ -4838,7 +4838,7 @@
         <v>233</v>
       </c>
       <c r="N28" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="O28" t="s">
         <v>234</v>
@@ -4894,7 +4894,7 @@
         <v>124</v>
       </c>
       <c r="N29" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="O29" t="s">
         <v>95</v>
@@ -4950,7 +4950,7 @@
         <v>124</v>
       </c>
       <c r="N30" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="O30" t="s">
         <v>245</v>
@@ -5006,7 +5006,7 @@
         <v>124</v>
       </c>
       <c r="N31" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="O31" t="s">
         <v>251</v>
@@ -5112,7 +5112,7 @@
         <v>263</v>
       </c>
       <c r="N33" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="O33" t="s">
         <v>264</v>
@@ -5218,7 +5218,7 @@
         <v>277</v>
       </c>
       <c r="N35" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="O35" t="s">
         <v>278</v>
@@ -5274,7 +5274,7 @@
         <v>284</v>
       </c>
       <c r="N36" t="s">
-        <v>940</v>
+        <v>938</v>
       </c>
       <c r="O36" t="s">
         <v>285</v>
@@ -5330,7 +5330,7 @@
         <v>291</v>
       </c>
       <c r="N37" s="1" t="s">
-        <v>925</v>
+        <v>1000</v>
       </c>
       <c r="O37" t="s">
         <v>292</v>
@@ -5442,7 +5442,7 @@
         <v>124</v>
       </c>
       <c r="N39" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
       <c r="O39" t="s">
         <v>307</v>
@@ -5554,7 +5554,7 @@
         <v>124</v>
       </c>
       <c r="N41" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
       <c r="O41" t="s">
         <v>320</v>
@@ -5610,7 +5610,7 @@
         <v>326</v>
       </c>
       <c r="N42" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="O42" t="s">
         <v>327</v>
@@ -5666,7 +5666,7 @@
         <v>124</v>
       </c>
       <c r="N43" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="O43" t="s">
         <v>330</v>
@@ -5772,7 +5772,7 @@
         <v>341</v>
       </c>
       <c r="N45" t="s">
-        <v>938</v>
+        <v>936</v>
       </c>
       <c r="O45" t="s">
         <v>342</v>
@@ -5984,7 +5984,7 @@
         <v>364</v>
       </c>
       <c r="N49" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
       <c r="O49" t="s">
         <v>365</v>
@@ -6040,7 +6040,7 @@
         <v>371</v>
       </c>
       <c r="N50" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="O50" t="s">
         <v>372</v>
@@ -6096,7 +6096,7 @@
         <v>380</v>
       </c>
       <c r="N51" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="O51" t="s">
         <v>381</v>
@@ -6152,7 +6152,7 @@
         <v>388</v>
       </c>
       <c r="N52" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="O52" t="s">
         <v>390</v>
@@ -6208,7 +6208,7 @@
         <v>395</v>
       </c>
       <c r="N53" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="O53" t="s">
         <v>396</v>
@@ -6264,7 +6264,7 @@
         <v>124</v>
       </c>
       <c r="N54" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="O54" t="s">
         <v>401</v>
@@ -6320,7 +6320,7 @@
         <v>404</v>
       </c>
       <c r="N55" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
       <c r="O55" t="s">
         <v>405</v>
@@ -6376,7 +6376,7 @@
         <v>410</v>
       </c>
       <c r="N56" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
       <c r="O56" t="s">
         <v>411</v>
@@ -6432,7 +6432,7 @@
         <v>124</v>
       </c>
       <c r="N57" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
       <c r="O57" t="s">
         <v>416</v>
@@ -6488,7 +6488,7 @@
         <v>124</v>
       </c>
       <c r="N58" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
       <c r="O58" t="s">
         <v>421</v>
@@ -6544,7 +6544,7 @@
         <v>425</v>
       </c>
       <c r="N59" t="s">
-        <v>941</v>
+        <v>939</v>
       </c>
       <c r="O59" t="s">
         <v>426</v>
@@ -6600,7 +6600,7 @@
         <v>430</v>
       </c>
       <c r="N60" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
       <c r="O60" t="s">
         <v>431</v>
@@ -6656,7 +6656,7 @@
         <v>438</v>
       </c>
       <c r="N61" t="s">
-        <v>943</v>
+        <v>941</v>
       </c>
       <c r="O61" t="s">
         <v>439</v>
@@ -6712,7 +6712,7 @@
         <v>124</v>
       </c>
       <c r="N62" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="O62" t="s">
         <v>444</v>
@@ -6768,7 +6768,7 @@
         <v>271</v>
       </c>
       <c r="N63" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
       <c r="O63" t="s">
         <v>451</v>
@@ -6824,7 +6824,7 @@
         <v>456</v>
       </c>
       <c r="N64" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
       <c r="O64" t="s">
         <v>457</v>
@@ -6980,7 +6980,7 @@
         <v>471</v>
       </c>
       <c r="N67" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
       <c r="O67" t="s">
         <v>472</v>
@@ -7092,7 +7092,7 @@
         <v>481</v>
       </c>
       <c r="N69" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
       <c r="O69" t="s">
         <v>482</v>
@@ -7148,7 +7148,7 @@
         <v>488</v>
       </c>
       <c r="N70" t="s">
-        <v>949</v>
+        <v>947</v>
       </c>
       <c r="O70" t="s">
         <v>489</v>
@@ -7204,7 +7204,7 @@
         <v>495</v>
       </c>
       <c r="N71" t="s">
-        <v>950</v>
+        <v>948</v>
       </c>
       <c r="O71" t="s">
         <v>496</v>
@@ -7260,7 +7260,7 @@
         <v>501</v>
       </c>
       <c r="N72" t="s">
-        <v>944</v>
+        <v>942</v>
       </c>
       <c r="O72" t="s">
         <v>502</v>
@@ -7316,7 +7316,7 @@
         <v>508</v>
       </c>
       <c r="N73" t="s">
-        <v>951</v>
+        <v>949</v>
       </c>
       <c r="O73" t="s">
         <v>509</v>
@@ -7372,7 +7372,7 @@
         <v>144</v>
       </c>
       <c r="N74" t="s">
-        <v>952</v>
+        <v>950</v>
       </c>
       <c r="O74" t="s">
         <v>514</v>
@@ -7428,7 +7428,7 @@
         <v>520</v>
       </c>
       <c r="N75" t="s">
-        <v>953</v>
+        <v>951</v>
       </c>
       <c r="O75" t="s">
         <v>521</v>
@@ -7484,7 +7484,7 @@
         <v>528</v>
       </c>
       <c r="N76" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
       <c r="O76" t="s">
         <v>529</v>
@@ -7540,7 +7540,7 @@
         <v>535</v>
       </c>
       <c r="N77" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
       <c r="O77" t="s">
         <v>536</v>
@@ -7596,7 +7596,7 @@
         <v>541</v>
       </c>
       <c r="N78" t="s">
-        <v>956</v>
+        <v>954</v>
       </c>
       <c r="O78" t="s">
         <v>542</v>
@@ -7652,7 +7652,7 @@
         <v>94</v>
       </c>
       <c r="N79" t="s">
-        <v>957</v>
+        <v>955</v>
       </c>
       <c r="O79" t="s">
         <v>548</v>
@@ -7708,7 +7708,7 @@
         <v>124</v>
       </c>
       <c r="N80" t="s">
-        <v>958</v>
+        <v>956</v>
       </c>
       <c r="O80" t="s">
         <v>553</v>
@@ -7764,7 +7764,7 @@
         <v>558</v>
       </c>
       <c r="N81" t="s">
-        <v>959</v>
+        <v>957</v>
       </c>
       <c r="O81" t="s">
         <v>559</v>
@@ -7873,7 +7873,7 @@
         <v>124</v>
       </c>
       <c r="N83" t="s">
-        <v>957</v>
+        <v>955</v>
       </c>
       <c r="O83" t="s">
         <v>571</v>
@@ -7929,7 +7929,7 @@
         <v>124</v>
       </c>
       <c r="N84" t="s">
-        <v>960</v>
+        <v>958</v>
       </c>
       <c r="O84" t="s">
         <v>575</v>
@@ -8038,7 +8038,7 @@
         <v>124</v>
       </c>
       <c r="N86" t="s">
-        <v>957</v>
+        <v>955</v>
       </c>
       <c r="O86" t="s">
         <v>585</v>
@@ -8091,7 +8091,7 @@
         <v>590</v>
       </c>
       <c r="N87" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
       <c r="O87" t="s">
         <v>591</v>
@@ -8147,7 +8147,7 @@
         <v>596</v>
       </c>
       <c r="N88" t="s">
-        <v>962</v>
+        <v>960</v>
       </c>
       <c r="O88" t="s">
         <v>597</v>
@@ -8203,7 +8203,7 @@
         <v>124</v>
       </c>
       <c r="N89" t="s">
-        <v>963</v>
+        <v>961</v>
       </c>
       <c r="O89" t="s">
         <v>600</v>
@@ -8259,7 +8259,7 @@
         <v>124</v>
       </c>
       <c r="N90" t="s">
-        <v>964</v>
+        <v>962</v>
       </c>
       <c r="O90" t="s">
         <v>605</v>
@@ -8315,7 +8315,7 @@
         <v>124</v>
       </c>
       <c r="N91" t="s">
-        <v>965</v>
+        <v>963</v>
       </c>
       <c r="O91" t="s">
         <v>611</v>
@@ -8371,7 +8371,7 @@
         <v>614</v>
       </c>
       <c r="N92" t="s">
-        <v>966</v>
+        <v>964</v>
       </c>
       <c r="O92" t="s">
         <v>615</v>
@@ -8427,7 +8427,7 @@
         <v>124</v>
       </c>
       <c r="N93" t="s">
-        <v>967</v>
+        <v>965</v>
       </c>
       <c r="O93" t="s">
         <v>621</v>
@@ -8483,7 +8483,7 @@
         <v>626</v>
       </c>
       <c r="N94" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="O94" t="s">
         <v>627</v>
@@ -8539,7 +8539,7 @@
         <v>124</v>
       </c>
       <c r="N95" t="s">
-        <v>969</v>
+        <v>967</v>
       </c>
       <c r="O95" t="s">
         <v>633</v>
@@ -8595,7 +8595,7 @@
         <v>639</v>
       </c>
       <c r="N96" t="s">
-        <v>970</v>
+        <v>968</v>
       </c>
       <c r="O96" t="s">
         <v>640</v>
@@ -8819,7 +8819,7 @@
         <v>666</v>
       </c>
       <c r="N100" t="s">
-        <v>971</v>
+        <v>969</v>
       </c>
       <c r="O100" t="s">
         <v>667</v>
@@ -8875,7 +8875,7 @@
         <v>124</v>
       </c>
       <c r="N101" t="s">
-        <v>972</v>
+        <v>970</v>
       </c>
       <c r="O101" t="s">
         <v>671</v>
@@ -8978,7 +8978,7 @@
         <v>124</v>
       </c>
       <c r="N103" t="s">
-        <v>973</v>
+        <v>971</v>
       </c>
       <c r="O103" t="s">
         <v>682</v>
@@ -9146,7 +9146,7 @@
         <v>702</v>
       </c>
       <c r="N106" t="s">
-        <v>974</v>
+        <v>972</v>
       </c>
       <c r="O106" t="s">
         <v>703</v>
@@ -9202,7 +9202,7 @@
         <v>708</v>
       </c>
       <c r="N107" t="s">
-        <v>975</v>
+        <v>973</v>
       </c>
       <c r="O107" t="s">
         <v>709</v>
@@ -9258,7 +9258,7 @@
         <v>715</v>
       </c>
       <c r="N108" t="s">
-        <v>976</v>
+        <v>974</v>
       </c>
       <c r="O108" t="s">
         <v>716</v>
@@ -9314,7 +9314,7 @@
         <v>124</v>
       </c>
       <c r="N109" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
       <c r="O109" t="s">
         <v>722</v>
@@ -9370,7 +9370,7 @@
         <v>729</v>
       </c>
       <c r="N110" t="s">
-        <v>977</v>
+        <v>975</v>
       </c>
       <c r="O110" t="s">
         <v>730</v>
@@ -9426,7 +9426,7 @@
         <v>735</v>
       </c>
       <c r="N111" t="s">
-        <v>978</v>
+        <v>976</v>
       </c>
       <c r="O111" t="s">
         <v>736</v>
@@ -9482,7 +9482,7 @@
         <v>695</v>
       </c>
       <c r="N112" t="s">
-        <v>979</v>
+        <v>977</v>
       </c>
       <c r="O112" t="s">
         <v>740</v>
@@ -9535,7 +9535,7 @@
         <v>745</v>
       </c>
       <c r="N113" t="s">
-        <v>980</v>
+        <v>978</v>
       </c>
       <c r="O113" t="s">
         <v>746</v>
@@ -9647,7 +9647,7 @@
         <v>759</v>
       </c>
       <c r="N115" t="s">
-        <v>981</v>
+        <v>979</v>
       </c>
       <c r="O115" t="s">
         <v>760</v>
@@ -9703,7 +9703,7 @@
         <v>763</v>
       </c>
       <c r="N116" t="s">
-        <v>982</v>
+        <v>980</v>
       </c>
       <c r="O116" t="s">
         <v>601</v>
@@ -9759,7 +9759,7 @@
         <v>271</v>
       </c>
       <c r="N117" t="s">
-        <v>983</v>
+        <v>981</v>
       </c>
       <c r="O117" t="s">
         <v>768</v>
@@ -9815,7 +9815,7 @@
         <v>773</v>
       </c>
       <c r="N118" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
       <c r="O118" t="s">
         <v>774</v>
@@ -9927,7 +9927,7 @@
         <v>787</v>
       </c>
       <c r="N120" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
       <c r="O120" t="s">
         <v>788</v>
@@ -9983,7 +9983,7 @@
         <v>793</v>
       </c>
       <c r="N121" t="s">
-        <v>986</v>
+        <v>984</v>
       </c>
       <c r="O121" t="s">
         <v>794</v>
@@ -10095,7 +10095,7 @@
         <v>806</v>
       </c>
       <c r="N123" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
       <c r="O123" t="s">
         <v>807</v>
@@ -10151,7 +10151,7 @@
         <v>124</v>
       </c>
       <c r="N124" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
       <c r="O124" t="s">
         <v>811</v>
@@ -10204,7 +10204,7 @@
         <v>816</v>
       </c>
       <c r="N125" t="s">
-        <v>991</v>
+        <v>989</v>
       </c>
       <c r="O125" t="s">
         <v>817</v>
@@ -10260,7 +10260,7 @@
         <v>821</v>
       </c>
       <c r="N126" t="s">
-        <v>989</v>
+        <v>987</v>
       </c>
       <c r="O126" t="s">
         <v>822</v>
@@ -10316,7 +10316,7 @@
         <v>124</v>
       </c>
       <c r="N127" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
       <c r="O127" t="s">
         <v>828</v>
@@ -10372,7 +10372,7 @@
         <v>225</v>
       </c>
       <c r="N128" t="s">
-        <v>992</v>
+        <v>990</v>
       </c>
       <c r="O128" t="s">
         <v>833</v>
@@ -10481,7 +10481,7 @@
         <v>844</v>
       </c>
       <c r="N130" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
       <c r="O130" t="s">
         <v>845</v>
@@ -10537,7 +10537,7 @@
         <v>430</v>
       </c>
       <c r="N131" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
       <c r="O131" t="s">
         <v>850</v>
@@ -10590,7 +10590,7 @@
         <v>854</v>
       </c>
       <c r="N132" t="s">
-        <v>995</v>
+        <v>993</v>
       </c>
       <c r="O132" t="s">
         <v>855</v>
@@ -10646,7 +10646,7 @@
         <v>860</v>
       </c>
       <c r="N133" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
       <c r="O133" t="s">
         <v>861</v>
@@ -10702,7 +10702,7 @@
         <v>865</v>
       </c>
       <c r="N134" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
       <c r="O134" t="s">
         <v>866</v>
@@ -10814,7 +10814,7 @@
         <v>877</v>
       </c>
       <c r="N136" t="s">
-        <v>998</v>
+        <v>996</v>
       </c>
       <c r="O136" t="s">
         <v>878</v>
@@ -10870,7 +10870,7 @@
         <v>124</v>
       </c>
       <c r="N137" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
       <c r="O137" t="s">
         <v>389</v>
@@ -10982,7 +10982,7 @@
         <v>124</v>
       </c>
       <c r="N139" t="s">
-        <v>1000</v>
+        <v>998</v>
       </c>
       <c r="O139" t="s">
         <v>893</v>

</xml_diff>